<commit_message>
updated metafor analysis file, acclimation paper added to database, new excel file for excluded data from metafor analysis
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /acclimation /acclimationjan29.xlsx
+++ b/data extraction /lit search metadata /acclimation /acclimationjan29.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /acclimation /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1033DDE-6A04-8F41-BD89-D5CF356F0B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557C6F7-CA2D-7048-BB28-A66EB35DE50B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="28600" windowHeight="14400" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
+    <workbookView xWindow="5520" yWindow="460" windowWidth="28600" windowHeight="14400" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>Bartheld_2017_JOOFTHBI</t>
   </si>
@@ -421,6 +421,36 @@
   </si>
   <si>
     <t>pulse press, acclimation experiment</t>
+  </si>
+  <si>
+    <t>Bernhardt_2018_PROFTHROSOB.SC</t>
+  </si>
+  <si>
+    <t>Bernhardt, Joey R. and Sunday, Jennifer M. and Thompson, Patrick L. and O'Connor, Mary I.</t>
+  </si>
+  <si>
+    <t>Nonlinear averaging of thermal experience predicts population growth rates in a thermally variable environment</t>
+  </si>
+  <si>
+    <t>PROCEEDINGS OF THE ROYAL SOCIETY B-BIOLOGICAL SCIENCES</t>
+  </si>
+  <si>
+    <t>10.1098/rspb.2018.1076</t>
+  </si>
+  <si>
+    <t>As thermal regimes change worldwide, projections of future population and species persistence often require estimates of how population growth rates depend on temperature. These projections rarely account for how temporal variation in temperature can systematically modify growth rates relative to projections based on constant temperatures. Here, we tested the hypothesis that time-averaged population growth rates in fluctuating thermal environments differ from growth rates in constant conditions as a consequence of Jensen's inequality, and that the thermal performance curves (TPCs) describing population growth in fluctuating environments can be predicted quantitatively based on TPCs generated in constant laboratory conditions. With experimental populations of the green alga Tetraselmis tetrahele, we show that nonlinear averaging techniques accurately predicted increased as well as decreased population growth rates in fluctuating thermal regimes relative to constant thermal regimes. We extrapolate from these results to project critical temperatures for population growth and persistence of 89 phytoplankton species in naturally variable thermal environments. These results advance our ability to predict population dynamics in the context of global change.</t>
+  </si>
+  <si>
+    <t>0962-8452</t>
+  </si>
+  <si>
+    <t>Nonlinear Averaging of Thermal Experience Predicts Population Growth Rates in a Thermally Variable Environment.</t>
+  </si>
+  <si>
+    <t>background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check supplementary info, constant vs flux </t>
   </si>
 </sst>
 </file>
@@ -780,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8F4095-DAD1-314E-93A6-2C3D1771AF66}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N13"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,6 +1564,62 @@
         <v>10</v>
       </c>
     </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14">
+        <v>2018</v>
+      </c>
+      <c r="G14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" t="s">
+        <v>140</v>
+      </c>
+      <c r="L14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q15" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reorganizing folder, adding in data from new SCOPUS search, merging metadata files for the three research areas
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /acclimation /acclimationjan29.xlsx
+++ b/data extraction /lit search metadata /acclimation /acclimationjan29.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /acclimation /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C557C6F7-CA2D-7048-BB28-A66EB35DE50B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28D0177-6E0F-F543-8E57-E07215D22A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="460" windowWidth="28600" windowHeight="14400" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
+    <workbookView xWindow="28800" yWindow="-28000" windowWidth="23560" windowHeight="10000" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="146">
   <si>
     <t>Bartheld_2017_JOOFTHBI</t>
   </si>
@@ -147,9 +147,6 @@
     <t xml:space="preserve">y </t>
   </si>
   <si>
-    <t>Kern_2015_PHYS</t>
-  </si>
-  <si>
     <t>Kern, Pippa and Cramp, Rebecca L. and Seebacher, Frank and Kazerouni, Ensiyeh Ghanizadeh and Franklin, Craig E.</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Plasticity of Protective Mechanisms Only Partially Explains Interactive Effects of Temperature and Uvr on Upper Thermal Limits.</t>
   </si>
   <si>
-    <t>figure 1, 2</t>
-  </si>
-  <si>
     <t>Manenti_2014_JOOFEVBI</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>extractable?</t>
   </si>
   <si>
-    <t xml:space="preserve">acclimated at fluctuating and exposed to different constant treatments </t>
-  </si>
-  <si>
     <t>Hallsson_2012_JOOFEVBI</t>
   </si>
   <si>
@@ -366,21 +357,12 @@
     <t xml:space="preserve">heatshock, acclimation to fluctuating temps then measured traits at constant temps </t>
   </si>
   <si>
-    <t>figure 2, 3, 4</t>
-  </si>
-  <si>
-    <t>heatshock assay--likely not usable for acclimation?</t>
-  </si>
-  <si>
     <t xml:space="preserve">usable </t>
   </si>
   <si>
     <t>n</t>
   </si>
   <si>
-    <t xml:space="preserve">appear to have constant, flux, red and white temp treatments; exlcuded because they were reared in flux but then measured in two different regimes, return for acclimation analysis -- this features multiple generations </t>
-  </si>
-  <si>
     <t>y?</t>
   </si>
   <si>
@@ -420,9 +402,6 @@
     <t>figure 1,2,3</t>
   </si>
   <si>
-    <t>pulse press, acclimation experiment</t>
-  </si>
-  <si>
     <t>Bernhardt_2018_PROFTHROSOB.SC</t>
   </si>
   <si>
@@ -451,6 +430,39 @@
   </si>
   <si>
     <t xml:space="preserve">check supplementary info, constant vs flux </t>
+  </si>
+  <si>
+    <t>figure 2,3,4,5</t>
+  </si>
+  <si>
+    <t>extraction notes</t>
+  </si>
+  <si>
+    <t>the developmental data for this study was included in the strict, full analysis but it sounds like they measured those traits after exposing the Ctmax and acclimation assays to that data may need to included in the acclimation assay instead of the original analysis; unsure about sample size...methods listed 7-9 as sample size for each of the traits/temps so i assumed the lower of the two...</t>
+  </si>
+  <si>
+    <t>Kern_2015_phys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heatshock assay--likely not usable for acclimation, excluded because mean temperature not the same for flux and constant trt </t>
+  </si>
+  <si>
+    <t>acclimated at fluctuating and exposed to different constant treatments, not sure how to handle the isolated thermoperiod trts (no supp info or explanation in the methods)</t>
+  </si>
+  <si>
+    <t>appear to have constant, flux, red and white temp treatments; exlcuded because they were reared in flux but then measured in two different regimes, return for acclimation analysis -- this features multiple generations-- generation time IS 25 day at 30 C</t>
+  </si>
+  <si>
+    <t>table 1</t>
+  </si>
+  <si>
+    <t>figure 2, 3</t>
+  </si>
+  <si>
+    <t>pulse press, acclimation experiment-- cold exposure probably better for pulse press?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figure 2, fig s6 </t>
   </si>
 </sst>
 </file>
@@ -466,7 +478,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +488,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,10 +510,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,15 +829,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8F4095-DAD1-314E-93A6-2C3D1771AF66}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -874,151 +893,160 @@
         <v>30</v>
       </c>
       <c r="S1" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="T1" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>2017</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="R2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2015</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2015</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="F4" s="2">
         <v>2015</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
@@ -1033,51 +1061,51 @@
         <v>10</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="F5" s="2">
         <v>2014</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>8</v>
@@ -1101,48 +1129,48 @@
         <v>13</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1">
         <v>2019</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>8</v>
@@ -1160,45 +1188,48 @@
         <v>13</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F7" s="1">
         <v>2012</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>8</v>
@@ -1210,107 +1241,113 @@
         <v>11</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>10</v>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2020</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G8" s="1" t="s">
+    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="F9" s="1">
         <v>2015</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>8</v>
@@ -1322,110 +1359,113 @@
         <v>11</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>118</v>
+      <c r="F10" s="3">
+        <v>2014</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2014</v>
-      </c>
-      <c r="G10" s="1" t="s">
+    <row r="11" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="R10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F11" s="2">
         <v>2017</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>8</v>
@@ -1437,187 +1477,187 @@
         <v>39</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="Q11" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2018</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>116</v>
+      <c r="H13" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="1">
+    <row r="14" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="3">
         <v>2018</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="G14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="S12" s="1" t="s">
+      <c r="O14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="S14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2016</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14">
-        <v>2018</v>
-      </c>
-      <c r="G14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H14" t="s">
-        <v>138</v>
-      </c>
-      <c r="I14" t="s">
-        <v>139</v>
-      </c>
-      <c r="J14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" t="s">
-        <v>140</v>
-      </c>
-      <c r="L14" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" t="s">
-        <v>10</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="Q15" s="1"/>
     </row>
   </sheetData>

</xml_diff>